<commit_message>
Implemented multi-threading for faster data collection
</commit_message>
<xml_diff>
--- a/reports/Product_Analysis_Report.xlsx
+++ b/reports/Product_Analysis_Report.xlsx
@@ -565,7 +565,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,841 +603,946 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dell - Latitude 3000 15.6" Laptop - Intel Core i7 with 16GB Memory - 512 GB SSD - Soft Charcoal, Other</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 14" 2K Touch - Screen Laptop - AMD Ryzen AI 5 - 16GB Memory - 512GB SSD - Meteor Silver</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1249.99</v>
+        <v>549.99</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 15.6" Touch Screen Laptop - AMD Ryzen 7 7730U with 16GB Memory - 1TB SSD - Black</t>
+          <t>HP - 15.6" Full HD Touch - Screen Laptop - Intel Core i7 - 16GB Memory - 512GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>549.99</v>
+        <v>529.99</v>
       </c>
       <c r="D3" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="E3" t="n">
-        <v>175</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 15" Touch Screen Laptop - Intel Core i7 with 16GB Memory - 1TB SSD - Black</t>
+          <t>HP - 17.3" Full HD Laptop - AMD Ryzen 5 - 8GB Memory - 512GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>799.99</v>
+        <v>329.99</v>
       </c>
       <c r="D4" t="n">
         <v>4.6</v>
       </c>
       <c r="E4" t="n">
-        <v>97</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dell - XPS 16 16.3” 120Hz Laptop 2K - Intel Core Ultra 7 Series 1 with 16GB Memory – NVIDIA GeForce RTX 4050 - 1TB SSD - Platinum</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 14" 2K Touch - Screen Laptop - AMD Ryzen AI 7 - 24GB Memory - 1TB SSD - Meteor Silver</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1399.99</v>
+        <v>699.99</v>
       </c>
       <c r="D5" t="n">
-        <v>4.4</v>
+        <v>4.6</v>
       </c>
       <c r="E5" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dell - Plus 2 - in - 1 16" FHD+ Touch Screen Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 1TB SSD - Ice</t>
+          <t>HP - 15.6" Touch - Screen Laptop - Intel Core i3 - 8GB Memory - 256GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1099.99</v>
+        <v>279.99</v>
       </c>
       <c r="D6" t="n">
         <v>4.7</v>
       </c>
       <c r="E6" t="n">
-        <v>104</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dell - Plus 16" FHD+ Touch Screen Laptop - AMD Ryzen AI 7 350 Copilot+ PC with 32GB Memory - 1TB SDD - Ice Blue</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 14" 2K Touch - Screen Laptop - AMD Ryzen AI 5 - 16GB Memory - 512GB SSD - Meteor Silver</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1099.99</v>
+        <v>549.99</v>
       </c>
       <c r="D7" t="n">
-        <v>4.4</v>
+        <v>4.7</v>
       </c>
       <c r="E7" t="n">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dell - XPS 13.4" OLED 3K Touch - Screen Laptop - Snapdragon X Elite Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
+          <t>HP - Victus 15.6" 144Hz Full HD Gaming Laptop - Intel Core i5 - 8GB Memory - NVIDIA GeForce RTX 3050 - 512GB SSD - Mica Silver</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>999.99</v>
+        <v>779.99</v>
       </c>
       <c r="D8" t="n">
-        <v>4.4</v>
+        <v>4.6</v>
       </c>
       <c r="E8" t="n">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dell - Plus 2 - in - 1 14" FHD+ Touch Screen Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 1TB SSD - Ice</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 14" 2K Touch - Screen Laptop - AMD Ryzen AI 7 - 24GB Memory - 1TB SSD - Meteor Silver</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>799.99</v>
+        <v>699.99</v>
       </c>
       <c r="D9" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="E9" t="n">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14" FHD+ Laptop - Snapdragon X Copilot+ PC with 16GB Memory - 512GB SSD - Titan</t>
+          <t>HP - Envy 2 - in - 1 14" Full HD Touch - Screen Laptop - Intel Core 7 - 16GB Memory - 512GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>799.99</v>
+        <v>599.99</v>
       </c>
       <c r="D10" t="n">
-        <v>4.8</v>
+        <v>4.6</v>
       </c>
       <c r="E10" t="n">
-        <v>23</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dell - XPS 13.4" OLED 3K Touch - Screen Laptop - Snapdragon X Elite Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 16" 2K Touch - Screen Laptop - Intel Core Ultra 5 - 16GB Memory - 512GB SSD - Eclipse Gray</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>999.99</v>
+        <v>649.99</v>
       </c>
       <c r="D11" t="n">
-        <v>4.4</v>
+        <v>4.9</v>
       </c>
       <c r="E11" t="n">
-        <v>161</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 2 - in - 1 16” IPS LED FHD Touch Screen Laptop - Intel Core Ultra 7 with 16GB Memory - 1TB SSD - Ice Blue</t>
+          <t>HP - 14" Laptop - Intel Processor N150 - 4GB Memory - 128GB UFS - Sky Blue</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>919.99</v>
+        <v>149.99</v>
       </c>
       <c r="D12" t="n">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="E12" t="n">
-        <v>843</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dell - G15 15.6" 120Hz Gaming Laptop FHD - Intel 13th Gen Core i7 with 16GB Memory - NVIDIA GeForce RTX 4060 - 1TB SSD - Dark Shadow Gray</t>
+          <t>HP - Envy 2 - in - 1 14" 2K Touch - Screen Laptop - Intel Core Ultra 7 - 32GB Memory - 1TB SSD - Meteor Silver</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>833.99</v>
+        <v>864.99</v>
       </c>
       <c r="D13" t="n">
         <v>4.6</v>
       </c>
       <c r="E13" t="n">
-        <v>236</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14 Plus 14" QHD Touch Screen Laptop - Snapdragon X Plus Copilot+ PC with 16GB Memory - 512GB SSD - Ice Blue</t>
+          <t>HP - OmniBook 5 Flip 2 - in - 1 14" 2K Touch - Screen Laptop - Intel Core 7 - 16GB Memory - 512GB SSD - Glacier Silver</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>999.99</v>
+        <v>799.99</v>
       </c>
       <c r="D14" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="E14" t="n">
-        <v>124</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 2 - in - 1 14” IPS LED FHD+ Touch Screen Laptop – Intel Core 7 with 16GB Memory – 1TB SSD - Ice Blue</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 16" 2K Touch - Screen Laptop - Intel Core Ultra 7 - 32GB Memory - 2TB SSD - Eclipse Gray</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>999.99</v>
+        <v>1049.99</v>
       </c>
       <c r="D15" t="n">
-        <v>4.6</v>
+        <v>4.9</v>
       </c>
       <c r="E15" t="n">
-        <v>777</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Dell - XPS 13 13.4” 2K Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
+          <t>HP - OmniBook X Flip 2 - in - 1 - Copilot+ PC - 16" 2K Touch - Screen Laptop - Intel Core Ultra 7 - 16GB Memory - 1TB SSD - Eclipse Gray</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1399.99</v>
+        <v>1099.99</v>
       </c>
       <c r="D16" t="n">
-        <v>4.4</v>
+        <v>4.8</v>
       </c>
       <c r="E16" t="n">
-        <v>69</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14 2 - in - 1 14" IPS LED FHD Touch Screen Laptop - AMD Ryzen 5 with 8GB Memory - 512GB SSD - Midnight Blue</t>
+          <t>HP - OmniBook Ultra Flip 2 - in - 1 - Copilot+ PC - 14" 3K OLED Touch - Screen Laptop - Intel Core Ultra 9 - 32G Memory - 2TB SSD - Eclipse Gray</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>656.99</v>
+        <v>1499.99</v>
       </c>
       <c r="D17" t="n">
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="E17" t="n">
-        <v>486</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14 Plus 14" QHD Touch Screen Laptop - Snapdragon X Plus Copilot+ PC with 16GB Memory - 512GB SSD - Ice Blue</t>
+          <t>HP - 15.6" Touch - Screen Laptop - AMD Ryzen 5 - 16GB Memory - 256GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>999.99</v>
+        <v>349.99</v>
       </c>
       <c r="D18" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="E18" t="n">
-        <v>124</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14 2 - in - 1 14" IPS LED Touch Screen Laptop - AMD Ryzen 7 with 16GB Memory - 1TB SSD - Midnight Blue</t>
+          <t>HP - Victus 15.6" 144Hz Full HD Gaming Laptop - Intel Core i5 - 8GB Memory - NVIDIA GeForce RTX 3050 - 512GB SSD - Mica Silver</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>949.99</v>
+        <v>779.99</v>
       </c>
       <c r="D19" t="n">
-        <v>4.5</v>
+        <v>4.6</v>
       </c>
       <c r="E19" t="n">
-        <v>272</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Dell - XPS 16 16.3” 120Hz Laptop 2K - Intel Core Ultra 7 Series 1 with 16GB Memory – NVIDIA GeForce RTX 4050 - 1TB SSD - Platinum</t>
+          <t>HP - 14" Laptop - Intel Celeron - 4GB Memory - 64GB eMMC - Snowflake White</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1399.99</v>
+        <v>199.99</v>
       </c>
       <c r="D20" t="n">
-        <v>4.4</v>
+        <v>4.2</v>
       </c>
       <c r="E20" t="n">
-        <v>61</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Dell - Plus 2 - In - 1 16" FHD+ Laptop - Intel Core Ultra 5 Copilot+ PC with 16GB Memory - 512GB SSD - Ice</t>
+          <t>HP - OmniBook 5 Flip 2 - in - 1 14" 2K Touch - Screen Laptop - Intel Core 7 - 16GB Memory - 512GB SSD - Glacier Silver</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>649.99</v>
+        <v>799.99</v>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Dell - Precision 3000 14" Laptop - Intel Core Ultra 5 with 16GB Memory - 256 GB SSD - Gray</t>
+          <t>HP - 17.3" HD+ Laptop - Intel Core i3 - 8GB Memory - 256GB SSD - Natural Silver</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1399.99</v>
+        <v>579.99</v>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Dell - Inspiron 14 2 - in - 1 14" Touch Screen Laptop - Intel Core 5 with 16GB Memory - 512GB SSD - Ice Blue</t>
+          <t>HP - 14" Chromebook - Intel Celeron - 4GB Memory - 64GB eMMC - Modern Grey</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>749.99</v>
+        <v>129</v>
       </c>
       <c r="D23" t="n">
-        <v>4.9</v>
+        <v>4.4</v>
       </c>
       <c r="E23" t="n">
-        <v>12</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M2 chip Built for Apple Intelligence - 16GB Memory - 256GB SSD - Midnight</t>
+          <t>HP - 15.6" Chromebook Laptop - Intel Processor N200 - 8GB Memory - 64GB eMMC - Natural Silver</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>699</v>
+        <v>179</v>
       </c>
       <c r="D24" t="n">
-        <v>4.9</v>
+        <v>4.5</v>
       </c>
       <c r="E24" t="n">
-        <v>1637</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 16GB Memory - 256GB SSD - Midnight</t>
+          <t>Dell - Latitude 3000 15.6" Laptop - Intel Core i7 with 16GB Memory - 512 GB SSD - Soft Charcoal, Other</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>849</v>
+        <v>1249.99</v>
       </c>
       <c r="D25" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="E25" t="n">
-        <v>1353</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 16GB Memory - 256GB SSD - Midnight</t>
+          <t>Dell - Inspiron 15" Touch Screen Laptop - Intel Core i5 with 8GB Memory - 512GB SSD - Black</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1049</v>
+        <v>349.99</v>
       </c>
       <c r="D26" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="E26" t="n">
-        <v>501</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Apple - MacBook Pro 14 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 16GB Memory - 512GB SSD - Space Black</t>
+          <t>Dell - Inspiron 15.6" Touch Screen Laptop - AMD Ryzen 7 7730U with 16GB Memory - 1TB SSD - Black</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1429</v>
+        <v>549.99</v>
       </c>
       <c r="D27" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="E27" t="n">
-        <v>1098</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - Apple M3 chip Built for Apple Intelligence - 16GB Memory - 256GB SSD - Starlight</t>
+          <t>Dell - XPS 16 16.3” 120Hz Laptop 2K - Intel Core Ultra 7 Series 1 with 16GB Memory – NVIDIA GeForce RTX 4050 - 1TB SSD - Platinum</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>899</v>
+        <v>1399.99</v>
       </c>
       <c r="D28" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="E28" t="n">
-        <v>588</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - M3 chip Built for Apple Intelligence - 16GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - Inspiron 15" Touch Screen Laptop - Intel Core i7 with 16GB Memory - 1TB SSD - Black</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>869.99</v>
+        <v>799.99</v>
       </c>
       <c r="D29" t="n">
-        <v>4.9</v>
+        <v>4.6</v>
       </c>
       <c r="E29" t="n">
-        <v>1302</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M3 chip Built for Apple Intelligence - 16GB Memory - 256GB SSD - Silver</t>
+          <t>Dell - Plus 2 - in - 1 16" FHD+ Touch Screen Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 1TB SSD - Ice</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>787.99</v>
+        <v>1099.99</v>
       </c>
       <c r="D30" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="E30" t="n">
-        <v>1455</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Geek Squad Certified Refurbished MacBook Air 13.6" Laptop - Apple M2 chip - 8GB Memory - 256GB SSD - Midnight</t>
+          <t>Dell - XPS 16" OLED Touch - Screen Laptop 4K - Intel Core Ultra 9 Series 1 with 32GB Memory - NVIDIA GeForce RTX 4060 - 1TB SSD - Platinum</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>599.99</v>
+        <v>3049.99</v>
       </c>
       <c r="D31" t="n">
-        <v>4.6</v>
+        <v>4.3</v>
       </c>
       <c r="E31" t="n">
-        <v>172</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Apple - MacBook Pro 14" Laptop - M3 Pro chip Built for Apple Intelligence - 18GB Memory - 14 - core GPU - 512GB SSD - Space Black</t>
+          <t>Dell - Plus 16" FHD+ Touch Screen Laptop - AMD Ryzen AI 7 350 Copilot+ PC with 32GB Memory - 1TB SDD - Ice Blue</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1286.99</v>
+        <v>1099.99</v>
       </c>
       <c r="D32" t="n">
-        <v>4.9</v>
+        <v>4.4</v>
       </c>
       <c r="E32" t="n">
-        <v>3189</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 16GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - Plus 2 - in - 1 14" FHD+ Touch Screen Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 1TB SSD - Ice</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1049</v>
+        <v>799.99</v>
       </c>
       <c r="D33" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="E33" t="n">
-        <v>390</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 16GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - Plus 2 - In - 1 16" Mini - LED Touch Screen Laptop - Intel Core Ultra 9 Copilot+ PC with 32GB Memory - 1TB SSD - Midnight</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1249</v>
+        <v>1599.99</v>
       </c>
       <c r="D34" t="n">
-        <v>4.9</v>
+        <v>4.6</v>
       </c>
       <c r="E34" t="n">
-        <v>214</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 24GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - Inspiron 14" FHD+ Laptop - Snapdragon X Copilot+ PC with 16GB Memory - 512GB SSD - Titan</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1449</v>
+        <v>799.99</v>
       </c>
       <c r="D35" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="E35" t="n">
-        <v>151</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M4 chip Built for Apple Intelligence - 24GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - XPS 13.4" OLED 3K Touch - Screen Laptop - Snapdragon X Elite Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1249</v>
+        <v>999.99</v>
       </c>
       <c r="D36" t="n">
-        <v>4.9</v>
+        <v>4.4</v>
       </c>
       <c r="E36" t="n">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Apple - MacBook Pro 14" Laptop - M3 chip Built for Apple Intelligence - 8GB Memory - 10 - core GPU - 1TB SSD - Space Gray</t>
+          <t>Dell - XPS 13.4" OLED 3K Touch - Screen Laptop - Snapdragon X Elite Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1161.99</v>
+        <v>999.99</v>
       </c>
       <c r="D37" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="E37" t="n">
-        <v>252</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - M3 chip Built for Apple Intelligence - 16GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - Inspiron 2 - in - 1 16” IPS LED FHD Touch Screen Laptop - Intel Core Ultra 7 with 16GB Memory - 1TB SSD - Ice Blue</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1099</v>
+        <v>919.99</v>
       </c>
       <c r="D38" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="E38" t="n">
-        <v>863</v>
+        <v>843</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - M3 chip Built for Apple Intelligence - 8GB Memory - 256GB SSD - Midnight</t>
+          <t>Dell - G15 15.6" 120Hz Gaming Laptop FHD - Intel 13th Gen Core i7 with 16GB Memory - NVIDIA GeForce RTX 4060 - 1TB SSD - Dark Shadow Gray</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>849</v>
+        <v>833.99</v>
       </c>
       <c r="D39" t="n">
-        <v>4.9</v>
+        <v>4.6</v>
       </c>
       <c r="E39" t="n">
-        <v>2217</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 15 - inch Laptop - M3 chip Built for Apple Intelligence - 8GB Memory - 256GB SSD - Midnight</t>
+          <t>Dell - Inspiron 2 - in - 1 14” IPS LED FHD+ Touch Screen Laptop – Intel Core 7 with 16GB Memory – 1TB SSD - Ice Blue</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>813.99</v>
+        <v>999.99</v>
       </c>
       <c r="D40" t="n">
-        <v>4.9</v>
+        <v>4.6</v>
       </c>
       <c r="E40" t="n">
-        <v>877</v>
+        <v>777</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Apple - MacBook Air 13 - inch Laptop - Apple M3 chip Built for Apple Intelligence - 24GB Memory - 512GB SSD - Midnight</t>
+          <t>Dell - XPS 13 13.4” 2K Laptop - Intel Core Ultra 7 Copilot+ PC with 16GB Memory - 512GB SSD - Graphite</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1033.99</v>
+        <v>1399.99</v>
       </c>
       <c r="D41" t="n">
-        <v>4.9</v>
+        <v>4.4</v>
       </c>
       <c r="E41" t="n">
-        <v>125</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Dell - Inspiron 14 2 - in - 1 14" IPS LED FHD Touch Screen Laptop - AMD Ryzen 5 with 8GB Memory - 512GB SSD - Midnight Blue</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>656.99</v>
+      </c>
+      <c r="D42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Dell - Inspiron 14 Plus 14" QHD Touch Screen Laptop - Snapdragon X Plus Copilot+ PC with 16GB Memory - 512GB SSD - Ice Blue</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>999.99</v>
+      </c>
+      <c r="D43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E43" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Dell - Inspiron 14 2 - in - 1 14" IPS LED Touch Screen Laptop - AMD Ryzen 7 with 16GB Memory - 1TB SSD - Midnight Blue</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>949.99</v>
+      </c>
+      <c r="D44" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E44" t="n">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Dell - XPS 16 16.3” 120Hz Laptop 2K - Intel Core Ultra 7 Series 1 with 16GB Memory – NVIDIA GeForce RTX 4050 - 1TB SSD - Platinum</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1399.99</v>
+      </c>
+      <c r="D45" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E45" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Dell - XPS 14 14.5" OLED 3.2K Touch - Screen Laptop – Intel Core Ultra 7 with 32GB Memory - 1TB SSD - Platinum</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>2099.99</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E46" t="n">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1484,33 +1589,33 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1023.55</v>
+        <v>1139.13</v>
       </c>
       <c r="C2" t="n">
-        <v>4.88</v>
+        <v>4.56</v>
       </c>
       <c r="D2" t="n">
-        <v>16540</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>989.13</v>
+        <v>615.34</v>
       </c>
       <c r="C3" t="n">
-        <v>4.62</v>
+        <v>4.63</v>
       </c>
       <c r="D3" t="n">
-        <v>3912</v>
+        <v>4970</v>
       </c>
     </row>
   </sheetData>

</xml_diff>